<commit_message>
Expanded emerging technologies considered
Added scripts to analyze and plot inputs for visual check
</commit_message>
<xml_diff>
--- a/projects/test_emerging_tech/data/data_emerging_tech.xlsx
+++ b/projects/test_emerging_tech/data/data_emerging_tech.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAF63B9-864A-4647-B795-D3AF7B0485C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B9502D-8795-400E-AAA8-17DEAFCEFA0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="941" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="87">
   <si>
     <t>connection</t>
   </si>
@@ -259,6 +259,33 @@
   </si>
   <si>
     <t>BIO_ATM</t>
+  </si>
+  <si>
+    <t>E_OCAES</t>
+  </si>
+  <si>
+    <t>E_SCO2</t>
+  </si>
+  <si>
+    <t>[hr]</t>
+  </si>
+  <si>
+    <t>NATGAS_CCS</t>
+  </si>
+  <si>
+    <t>NATGAS_TAXED</t>
+  </si>
+  <si>
+    <t>NATGAS_TO_CCS</t>
+  </si>
+  <si>
+    <t>E_PV_DIST_RES</t>
+  </si>
+  <si>
+    <t>SOLAR</t>
+  </si>
+  <si>
+    <t>ELC_DIST</t>
   </si>
 </sst>
 </file>
@@ -332,7 +359,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -623,16 +664,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
@@ -760,35 +802,52 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>-45.27</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
         <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="L5">
         <v>-100</v>
       </c>
     </row>
@@ -803,7 +862,7 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1069,15 +1128,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:H4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -1146,25 +1205,25 @@
         <v>61</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>52</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>53</v>
@@ -1181,25 +1240,25 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>53</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>52</v>
@@ -1209,38 +1268,111 @@
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="J5" s="2">
+        <v>24</v>
+      </c>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="A6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D3:H3">
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+  <conditionalFormatting sqref="D6:H6">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:H4">
+  <conditionalFormatting sqref="D7:H7">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:H5">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:H5">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -1252,15 +1384,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
@@ -1328,35 +1460,82 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>74</v>
+      <c r="A3" t="s">
+        <v>84</v>
       </c>
       <c r="B3" s="5">
-        <v>61.9</v>
+        <v>24</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5">
-        <v>35.299999999999997</v>
+        <v>25</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
-      <c r="H3" s="6">
-        <v>45</v>
+      <c r="H3" s="5">
+        <v>20</v>
       </c>
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5">
+        <v>50</v>
+      </c>
+      <c r="D5">
+        <v>80</v>
+      </c>
+      <c r="H5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="5">
+        <v>61.9</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6">
+        <v>45</v>
+      </c>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B7" s="5">
         <v>61.9</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D7" s="5">
         <v>35.299999999999997</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H7" s="6">
         <v>45</v>
       </c>
     </row>
@@ -1368,15 +1547,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J4"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
@@ -1385,6 +1564,8 @@
     <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1465,46 +1646,96 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="6">
-        <v>4020</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6">
-        <v>123</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="6">
-        <v>1.39</v>
-      </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="7"/>
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3000</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4">
+        <v>1000</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5">
+        <v>1600</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="6">
+        <v>4020</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6">
+        <v>123</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="6">
+        <v>1.39</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B7" s="6">
         <v>4020</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6">
+      <c r="C7" s="6"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6">
         <v>123</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="6">
+      <c r="F7" s="6"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="6">
         <v>1.39</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1514,15 +1745,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
@@ -1598,14 +1829,33 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Starting to add Monte Carlo simulation to emerging_tech project
</commit_message>
<xml_diff>
--- a/projects/test_emerging_tech/data/data_emerging_tech.xlsx
+++ b/projects/test_emerging_tech/data/data_emerging_tech.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B9502D-8795-400E-AAA8-17DEAFCEFA0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E76EF4-BAD9-4CD6-910A-D98226F7EF91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="941" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="941" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connections" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="100">
   <si>
     <t>connection</t>
   </si>
@@ -286,16 +286,56 @@
   </si>
   <si>
     <t>ELC_DIST</t>
+  </si>
+  <si>
+    <t>NREL ATB</t>
+  </si>
+  <si>
+    <t>NREL TP-6A20-65298</t>
+  </si>
+  <si>
+    <t>NREL ATB, Similar Lat as Kansas City</t>
+  </si>
+  <si>
+    <t>NREL ATB, Gas-CC-CC</t>
+  </si>
+  <si>
+    <t>99.9% capture</t>
+  </si>
+  <si>
+    <t>Projection</t>
+  </si>
+  <si>
+    <t>Discuss</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>To update</t>
+  </si>
+  <si>
+    <t>Same as offshore shallow wind</t>
+  </si>
+  <si>
+    <t>Brown et al., discuss</t>
+  </si>
+  <si>
+    <t>Not currently available</t>
+  </si>
+  <si>
+    <t>Currently available</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,8 +357,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,6 +382,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -341,10 +401,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -355,8 +416,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -667,7 +735,7 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -813,8 +881,12 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="L3">
-        <v>-45.27</v>
+      <c r="L3" s="12">
+        <f>50.3*-0.999</f>
+        <v>-50.249699999999997</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -859,10 +931,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -994,12 +1066,14 @@
         <v>69</v>
       </c>
       <c r="B3" s="2">
-        <v>2</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>97</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1017,6 +1091,9 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
+      <c r="Q3" s="12" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
@@ -1120,6 +1197,11 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
     </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="M15">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1131,7 +1213,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1387,7 +1469,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1464,46 +1546,72 @@
         <v>84</v>
       </c>
       <c r="B3" s="5">
-        <v>24</v>
-      </c>
-      <c r="C3" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="D3" s="5">
         <v>25</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5">
-        <v>20</v>
-      </c>
-      <c r="I3" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B4">
-        <v>50</v>
-      </c>
-      <c r="D4">
-        <v>50</v>
-      </c>
-      <c r="H4">
-        <v>30</v>
+      <c r="B4" s="2">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="12">
+        <v>7530</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H4" s="2">
+        <v>55</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>50</v>
       </c>
-      <c r="D5">
-        <v>80</v>
-      </c>
-      <c r="H5">
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="14">
+        <v>75</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="2">
         <v>25</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1511,32 +1619,47 @@
         <v>74</v>
       </c>
       <c r="B6" s="5">
-        <v>61.9</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5">
-        <v>35.299999999999997</v>
-      </c>
+        <v>60.6</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="F6" s="5">
+        <v>13500</v>
+      </c>
+      <c r="G6" t="s">
+        <v>87</v>
+      </c>
       <c r="H6" s="6">
         <v>45</v>
       </c>
-      <c r="I6" s="5"/>
+      <c r="I6" s="5" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B7" s="5">
-        <v>61.9</v>
-      </c>
-      <c r="D7" s="5">
-        <v>35.299999999999997</v>
+        <v>60.6</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="13">
+        <v>18</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="H7" s="6">
         <v>45</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1550,13 +1673,13 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
@@ -1650,20 +1773,30 @@
         <v>84</v>
       </c>
       <c r="B3" s="2">
-        <v>3000</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+        <v>3054</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-5.6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="E3" s="2">
-        <v>5</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="F3" s="2">
+        <v>-5.3</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="H3" s="2">
         <v>0</v>
       </c>
       <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="J3" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
     </row>
@@ -1671,28 +1804,64 @@
       <c r="A4" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B4">
-        <v>1000</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
+      <c r="B4" s="2">
+        <v>2778</v>
+      </c>
+      <c r="C4">
+        <v>-1.1499999999999999</v>
+      </c>
+      <c r="D4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="2">
+        <v>27</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1.67</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B5">
-        <v>1600</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
+      <c r="B5" s="2">
+        <v>1457</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="2">
+        <v>16.3</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2.57</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -1700,10 +1869,14 @@
         <v>74</v>
       </c>
       <c r="B6" s="6">
-        <v>4020</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="5"/>
+        <v>4309.3900000000003</v>
+      </c>
+      <c r="C6" s="6">
+        <v>-0.46</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="E6" s="6">
         <v>123</v>
       </c>
@@ -1713,27 +1886,37 @@
         <v>1.39</v>
       </c>
       <c r="I6" s="6"/>
-      <c r="J6" s="7"/>
+      <c r="J6" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="6">
-        <v>4020</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="5"/>
+      <c r="B7" s="11">
+        <v>7042.9497903138645</v>
+      </c>
+      <c r="C7" s="6">
+        <v>-0.72</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>92</v>
+      </c>
       <c r="E7" s="6">
-        <v>123</v>
+        <v>178.35</v>
       </c>
       <c r="F7" s="6"/>
-      <c r="G7" s="7"/>
+      <c r="G7" s="10" t="s">
+        <v>93</v>
+      </c>
       <c r="H7" s="6">
-        <v>1.39</v>
+        <v>3.82</v>
       </c>
       <c r="I7" s="6"/>
-      <c r="J7" s="7"/>
+      <c r="J7" s="7" t="s">
+        <v>92</v>
+      </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
@@ -1747,8 +1930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1832,20 +2015,43 @@
       <c r="A3" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="D3" s="2">
+        <v>28500</v>
+      </c>
+      <c r="E3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>78</v>
       </c>
+      <c r="D5">
+        <v>5000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
@@ -1853,10 +2059,20 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>75</v>
+      </c>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>